<commit_message>
working config file and persistent hard drive
</commit_message>
<xml_diff>
--- a/instruction_set.xlsx
+++ b/instruction_set.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\0x\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44E3DDF4-4A04-4A27-AEC4-047747D61555}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7992FD01-6038-4097-ABB2-7ED2C0739FEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2970" yWindow="1740" windowWidth="23025" windowHeight="14025" xr2:uid="{1E484941-6C4F-4B8C-8513-72E5850C2E1E}"/>
+    <workbookView xWindow="-25290" yWindow="2370" windowWidth="23025" windowHeight="14025" xr2:uid="{1E484941-6C4F-4B8C-8513-72E5850C2E1E}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -1518,8 +1518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48C68D6B-92A2-4BB8-9A39-79A2CDD34874}">
   <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>